<commit_message>
made changes into excel
</commit_message>
<xml_diff>
--- a/intern/excel/INT_2025.xlsx
+++ b/intern/excel/INT_2025.xlsx
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1080,7 @@
         <v>39</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>44</v>
@@ -2206,8 +2206,8 @@
       <c r="I27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>15</v>
+      <c r="J27" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
changes into excel and main.py
</commit_message>
<xml_diff>
--- a/intern/excel/INT_2025.xlsx
+++ b/intern/excel/INT_2025.xlsx
@@ -884,7 +884,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>44</v>

</xml_diff>